<commit_message>
improved flow of program
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencersedano/Desktop/2025 Coding Resolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4BEF62-3828-C24B-BA41-E218CEB7075B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6606F7-7EF5-6B47-821E-62A496224870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" xr2:uid="{44AB305C-C398-274B-AEE2-994E818B9269}"/>
+    <workbookView xWindow="160" yWindow="900" windowWidth="29920" windowHeight="18580" xr2:uid="{44AB305C-C398-274B-AEE2-994E818B9269}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="125">
   <si>
     <t>Week</t>
   </si>
@@ -62,18 +62,9 @@
     <t>Basic arithmetic operations with error handling.</t>
   </si>
   <si>
-    <t>Unit Converter</t>
-  </si>
-  <si>
-    <t>Length, weight, and temperature conversions.</t>
-  </si>
-  <si>
     <t>Personal Budget Tracker</t>
   </si>
   <si>
-    <t>Track income, expenses, and savings in a console app.</t>
-  </si>
-  <si>
     <t>Console-Based To-Do List</t>
   </si>
   <si>
@@ -411,6 +402,18 @@
   </si>
   <si>
     <t>Add GUI</t>
+  </si>
+  <si>
+    <t>Make it a blazor app</t>
+  </si>
+  <si>
+    <t>BMI Calculator</t>
+  </si>
+  <si>
+    <t>Weight and height to BMI</t>
+  </si>
+  <si>
+    <t>Track expenses, and savings in a console app.</t>
   </si>
 </sst>
 </file>
@@ -469,38 +472,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -522,26 +494,13 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -877,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B4DB55-BE55-E04B-9154-66CDC440505F}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:D29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -905,13 +864,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -928,10 +887,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
         <v>120</v>
-      </c>
-      <c r="F2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -942,12 +901,17 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1"/>
+        <v>123</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -957,10 +921,13 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>124</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,10 +938,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,13 +949,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -996,13 +963,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1010,13 +977,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1024,13 +991,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1038,13 +1005,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1052,13 +1019,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1066,13 +1033,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1080,13 +1047,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1094,13 +1061,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1108,13 +1075,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1122,13 +1089,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1136,13 +1103,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1150,13 +1117,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1164,13 +1131,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1178,13 +1145,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1192,13 +1159,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1206,13 +1173,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1220,13 +1187,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1234,13 +1201,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1248,13 +1215,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1262,13 +1229,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1276,13 +1243,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
         <v>58</v>
       </c>
-      <c r="C27" t="s">
-        <v>61</v>
-      </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1290,13 +1257,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1304,13 +1271,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,13 +1285,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1332,13 +1299,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1346,13 +1313,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1360,13 +1327,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1374,13 +1341,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1388,13 +1355,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
         <v>76</v>
       </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1402,13 +1369,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,13 +1383,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1430,13 +1397,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1444,13 +1411,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
         <v>85</v>
       </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1458,13 +1425,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1472,13 +1439,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D41" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1486,13 +1453,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D42" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,13 +1467,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
         <v>94</v>
       </c>
-      <c r="C43" t="s">
-        <v>97</v>
-      </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1514,13 +1481,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1528,13 +1495,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1542,13 +1509,13 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1556,13 +1523,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C47" t="s">
         <v>103</v>
       </c>
-      <c r="C47" t="s">
-        <v>106</v>
-      </c>
       <c r="D47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1570,13 +1537,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1584,13 +1551,13 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1598,13 +1565,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1612,13 +1579,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1626,13 +1593,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1640,37 +1607,27 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E50 F2">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"finished"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"on hold"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
+  <conditionalFormatting sqref="E3:F3">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"not started"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"on hold"</formula>
+  <conditionalFormatting sqref="F2:F3 E2:E50">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+      <formula>"finished"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E53 F2">
+  <conditionalFormatting sqref="F2:F3 E2:E53">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"on hold"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update Hoverzi and create Parser
</commit_message>
<xml_diff>
--- a/Timeline.xlsx
+++ b/Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencersedano/Desktop/2025 Coding Resolution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762EAB73-BB51-294C-89E4-3E32EAB4C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4227E1A7-91A9-B34B-A23E-344F9CD0F2C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="900" windowWidth="29920" windowHeight="18580" xr2:uid="{44AB305C-C398-274B-AEE2-994E818B9269}"/>
+    <workbookView xWindow="4680" yWindow="900" windowWidth="25800" windowHeight="18580" xr2:uid="{44AB305C-C398-274B-AEE2-994E818B9269}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="128">
   <si>
     <t>Week</t>
   </si>
@@ -74,12 +74,6 @@
     <t>Your first REST API.</t>
   </si>
   <si>
-    <t>Weather Dashboard</t>
-  </si>
-  <si>
-    <t>Fetch real-time weather data using APIs.</t>
-  </si>
-  <si>
     <t>Employee Management System</t>
   </si>
   <si>
@@ -423,6 +417,12 @@
   </si>
   <si>
     <t>Add validation and ASP.NET backend</t>
+  </si>
+  <si>
+    <t>CC-CEDICT Parser</t>
+  </si>
+  <si>
+    <t>Read files with C# and parse them into JSON</t>
   </si>
 </sst>
 </file>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B4DB55-BE55-E04B-9154-66CDC440505F}">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -873,10 +873,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -894,10 +894,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
         <v>113</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -908,16 +908,16 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -931,10 +931,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -945,16 +945,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" t="s">
         <v>120</v>
-      </c>
-      <c r="D5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -971,7 +971,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -982,16 +982,16 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
         <v>124</v>
       </c>
-      <c r="D7" t="s">
-        <v>126</v>
-      </c>
       <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
         <v>125</v>
-      </c>
-      <c r="F7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1002,10 +1002,13 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>127</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1024,10 +1027,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1035,13 +1038,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
         <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1049,13 +1052,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1063,13 +1066,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1077,13 +1080,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1091,13 +1094,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1105,13 +1108,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1119,13 +1122,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1133,13 +1136,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1147,13 +1150,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
         <v>33</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1161,13 +1164,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1175,13 +1178,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1189,13 +1192,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1203,13 +1206,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
         <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1217,13 +1220,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1231,13 +1234,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1245,13 +1248,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1259,13 +1262,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
         <v>51</v>
-      </c>
-      <c r="C27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1273,13 +1276,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1287,13 +1290,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1301,13 +1304,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1315,13 +1318,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
         <v>60</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1329,13 +1332,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1343,13 +1346,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1357,13 +1360,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1371,13 +1374,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
         <v>69</v>
-      </c>
-      <c r="C35" t="s">
-        <v>70</v>
-      </c>
-      <c r="D35" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1385,13 +1388,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1399,13 +1402,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1413,13 +1416,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1427,13 +1430,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" t="s">
         <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1441,13 +1444,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1455,13 +1458,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1469,13 +1472,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1483,13 +1486,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43" t="s">
+        <v>86</v>
+      </c>
+      <c r="D43" t="s">
         <v>87</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1497,13 +1500,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1511,13 +1514,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1525,13 +1528,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,13 +1542,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" t="s">
         <v>96</v>
-      </c>
-      <c r="C47" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1553,13 +1556,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1567,13 +1570,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1581,13 +1584,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1595,13 +1598,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1609,13 +1612,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,13 +1626,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1637,13 +1640,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>